<commit_message>
v2 recorde, file, canvas, screen
</commit_message>
<xml_diff>
--- a/RTC MultiConnection/proto/성능 테스트.xlsx
+++ b/RTC MultiConnection/proto/성능 테스트.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lee\study\Test-WebRtc\RTC MultiConnection\proto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681BB57A-BF6B-4B6E-A14E-6626271F3611}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A02227F-727B-4277-875C-0A1ED0EC0623}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4005" yWindow="2370" windowWidth="21585" windowHeight="11370" xr2:uid="{B999A838-1D08-4BBF-A85E-569F8CFFA738}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B999A838-1D08-4BBF-A85E-569F8CFFA738}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>